<commit_message>
Se termina de programar horario, quedando pendiente un bug del calendario
</commit_message>
<xml_diff>
--- a/data/datos.xlsx
+++ b/data/datos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="30">
   <si>
     <t>Horas</t>
   </si>
@@ -52,6 +52,9 @@
     <t>Estudio</t>
   </si>
   <si>
+    <t>Descanso</t>
+  </si>
+  <si>
     <t>8:00 - 9:00</t>
   </si>
   <si>
@@ -70,10 +73,16 @@
     <t>13:00 - 14:00</t>
   </si>
   <si>
-    <t>14:00 - 15:00</t>
-  </si>
-  <si>
-    <t>15:00 - 16:00</t>
+    <t>14:00 - 14:12</t>
+  </si>
+  <si>
+    <t>14:12 - 15:00</t>
+  </si>
+  <si>
+    <t>15:00 - 15:12</t>
+  </si>
+  <si>
+    <t>15:12 - 16:00</t>
   </si>
   <si>
     <t>16:00 - 17:00</t>
@@ -426,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -460,30 +469,12 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -506,7 +497,19 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -517,106 +520,128 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se termina proyecto, queda pendiente revisar pep8
</commit_message>
<xml_diff>
--- a/data/datos.xlsx
+++ b/data/datos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="33">
   <si>
     <t>Horas</t>
   </si>
@@ -46,15 +46,15 @@
     <t>Clases</t>
   </si>
   <si>
+    <t>Estudio</t>
+  </si>
+  <si>
+    <t>Descanso</t>
+  </si>
+  <si>
     <t>Ocio</t>
   </si>
   <si>
-    <t>Estudio</t>
-  </si>
-  <si>
-    <t>Descanso</t>
-  </si>
-  <si>
     <t>8:00 - 9:00</t>
   </si>
   <si>
@@ -67,22 +67,31 @@
     <t>11:00 - 12:00</t>
   </si>
   <si>
-    <t>12:00 - 13:00</t>
-  </si>
-  <si>
-    <t>13:00 - 14:00</t>
-  </si>
-  <si>
-    <t>14:00 - 14:12</t>
-  </si>
-  <si>
-    <t>14:12 - 15:00</t>
-  </si>
-  <si>
-    <t>15:00 - 15:12</t>
-  </si>
-  <si>
-    <t>15:12 - 16:00</t>
+    <t>12:00 - 12:30</t>
+  </si>
+  <si>
+    <t>12:30 - 13:00</t>
+  </si>
+  <si>
+    <t>13:00 - 13:30</t>
+  </si>
+  <si>
+    <t>13:30 - 13:42</t>
+  </si>
+  <si>
+    <t>13:42 - 14:00</t>
+  </si>
+  <si>
+    <t>14:00 - 14:30</t>
+  </si>
+  <si>
+    <t>14:30 - 14:42</t>
+  </si>
+  <si>
+    <t>14:42 - 15:00</t>
+  </si>
+  <si>
+    <t>15:00 - 16:00</t>
   </si>
   <si>
     <t>16:00 - 17:00</t>
@@ -435,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -499,45 +508,33 @@
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>17</v>
       </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -545,22 +542,31 @@
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" t="s">
-        <v>12</v>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="F9" t="s">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -568,16 +574,40 @@
       <c r="A10" t="s">
         <v>21</v>
       </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>22</v>
       </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>23</v>
       </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
@@ -603,45 +633,60 @@
       <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>29</v>
       </c>
-      <c r="B18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" t="s">
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>